<commit_message>
Standardized colors and adding wide data
</commit_message>
<xml_diff>
--- a/data/chiropractic_care.xlsx
+++ b/data/chiropractic_care.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\BYUI_M221_Book_R\docs\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB5FA422-3387-4C67-9863-A272CF510B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA10178-5ADC-43AA-AE2A-29AB1A2C6D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50595" yWindow="-3825" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-52110" yWindow="-4830" windowWidth="21600" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,9 +39,6 @@
     <t>Europe</t>
   </si>
   <si>
-    <t>Preventative Health</t>
-  </si>
-  <si>
     <t>At Risk</t>
   </si>
   <si>
@@ -87,6 +82,9 @@
   </si>
   <si>
     <t>The Journal of the Canadian Chiropractic Association, 52(3), 175–184.</t>
+  </si>
+  <si>
+    <t>Prevention</t>
   </si>
 </sst>
 </file>
@@ -475,16 +473,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -498,12 +496,12 @@
         <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -512,12 +510,12 @@
         <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -528,7 +526,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -537,12 +535,12 @@
         <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -551,7 +549,7 @@
         <v>142</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -559,35 +557,35 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>75</v>
@@ -595,10 +593,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>82</v>
@@ -606,10 +604,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C11" s="1">
         <v>170</v>
@@ -620,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1">
         <v>85</v>
@@ -628,10 +626,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
         <v>97</v>
@@ -639,10 +637,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <v>82</v>
@@ -650,10 +648,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1">
         <v>111</v>
@@ -661,10 +659,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1">
         <v>178</v>
@@ -674,28 +672,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revised Data for consistency
</commit_message>
<xml_diff>
--- a/data/chiropractic_care.xlsx
+++ b/data/chiropractic_care.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA7F1E50-ECC4-43D3-B66E-F9A366E31688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A63010-FFA2-4F2E-82CB-E162BF85CE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23520" yWindow="-4020" windowWidth="14400" windowHeight="7365"/>
+    <workbookView xWindow="-23910" yWindow="-2490" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chiropractic_care.xlsx" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,9 +43,6 @@
     <t>Charles Blum, Gary Globe, Lisa Terre, Timothy A. Mirtz, Leon Greene, and Denise Globe.</t>
   </si>
   <si>
-    <t>Preventative Health</t>
-  </si>
-  <si>
     <t>Multinational survey of chiropractic patients: reasons for seeking care. Journal of the Canadian</t>
   </si>
   <si>
@@ -65,12 +74,15 @@
   </si>
   <si>
     <t>source</t>
+  </si>
+  <si>
+    <t>Preventative</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -904,25 +916,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -944,13 +956,13 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -958,13 +970,13 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -972,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>77</v>
@@ -983,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>95</v>
@@ -991,7 +1003,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -1002,10 +1014,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>59</v>
@@ -1013,10 +1025,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>83</v>
@@ -1024,10 +1036,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>68</v>
@@ -1035,10 +1047,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>188</v>
@@ -1046,7 +1058,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -1057,10 +1069,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>76</v>
@@ -1068,10 +1080,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>65</v>
@@ -1079,10 +1091,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>82</v>
@@ -1090,10 +1102,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>252</v>

</xml_diff>

<commit_message>
Revised Prevention or Preventative Health to Prevention
</commit_message>
<xml_diff>
--- a/data/chiropractic_care.xlsx
+++ b/data/chiropractic_care.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A63010-FFA2-4F2E-82CB-E162BF85CE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D8CC69-1E3B-4A1A-AE3D-12D1E4F1F375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23910" yWindow="-2490" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24420" yWindow="-3000" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chiropractic_care.xlsx" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
     <t>source</t>
   </si>
   <si>
-    <t>Preventative</t>
+    <t>Prevention</t>
   </si>
 </sst>
 </file>

</xml_diff>